<commit_message>
Data update May 18, 2020
</commit_message>
<xml_diff>
--- a/COVID19_Deutschland.xlsx
+++ b/COVID19_Deutschland.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="158">
   <si>
     <t>Untere Grenze des 95%-Prädiktionsintervalls der Anzahl Neuerkrankungen</t>
   </si>
@@ -478,20 +478,32 @@
     <t>AS</t>
   </si>
   <si>
-    <t>Preprint, 17.5.2020</t>
-  </si>
-  <si>
     <t>bis 12.5., nicht verändern!</t>
   </si>
   <si>
     <t>Excel-Tabelle zum Nowcasting vom 17.5.2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preprint, 17.5.2020, Karlsruher Institut für Technologie, Researchgate, </t>
+  </si>
+  <si>
+    <t>https://publikationen.bibliothek.kit.edu/1000119466/7364762</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.13140/RG.2.2.14990</t>
+  </si>
+  <si>
+    <t>täglich</t>
+  </si>
+  <si>
+    <t>reguläre Datenupdates</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -520,6 +532,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -565,14 +583,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -694,8 +713,10 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="4"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="5"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
+    <cellStyle name="Link" xfId="5" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="1"/>
     <cellStyle name="Standard 3" xfId="2"/>
@@ -2575,7 +2596,7 @@
         <v>1123</v>
       </c>
       <c r="AQ16" s="15">
-        <f t="shared" ref="AQ16:AQ74" si="20">ABS(P16-$D16)</f>
+        <f t="shared" ref="AQ16:AQ73" si="20">ABS(P16-$D16)</f>
         <v>1884.2857142857147</v>
       </c>
       <c r="AR16" s="15">
@@ -2907,7 +2928,7 @@
         <v>4986.8571428571431</v>
       </c>
       <c r="Q19" s="15">
-        <f t="shared" ref="Q19:Q73" si="21">P20/P16</f>
+        <f t="shared" ref="Q19:Q72" si="21">P20/P16</f>
         <v>1.2359961368653423</v>
       </c>
       <c r="R19" s="12">
@@ -5033,15 +5054,15 @@
         <v>3.3567870715419001E-2</v>
       </c>
       <c r="AM34" s="15">
-        <f t="shared" ref="AM34:AM74" si="24">ABS(AC34-$M34)</f>
+        <f t="shared" ref="AM34:AM73" si="24">ABS(AC34-$M34)</f>
         <v>1.738406247840496E-2</v>
       </c>
       <c r="AN34" s="15">
-        <f t="shared" ref="AN34:AN74" si="25">ABS(X34-$M34)</f>
+        <f t="shared" ref="AN34:AN73" si="25">ABS(X34-$M34)</f>
         <v>0.37</v>
       </c>
       <c r="AO34" s="15">
-        <f t="shared" ref="AO34:AO75" si="26">ABS(AG34-$M34)</f>
+        <f t="shared" ref="AO34:AO73" si="26">ABS(AG34-$M34)</f>
         <v>4.7403016348779636E-2</v>
       </c>
       <c r="AP34" s="15">
@@ -7147,7 +7168,7 @@
         <v>6.9231356814170475E-2</v>
       </c>
       <c r="AP47" s="15">
-        <f t="shared" ref="AP47:AP75" si="33">ABS(G47-$D47)</f>
+        <f t="shared" ref="AP47:AP74" si="33">ABS(G47-$D47)</f>
         <v>130</v>
       </c>
       <c r="AQ47" s="15">
@@ -7159,7 +7180,7 @@
         <v>49.85714285714289</v>
       </c>
       <c r="AS47" s="15">
-        <f t="shared" ref="AS47:AS75" si="35">ABS(AB47-$D47)</f>
+        <f t="shared" ref="AS47:AS74" si="35">ABS(AB47-$D47)</f>
         <v>127.52136820896544</v>
       </c>
     </row>
@@ -11298,7 +11319,7 @@
       <c r="AH73" s="39"/>
       <c r="AI73" s="38"/>
       <c r="AJ73" s="15">
-        <f t="shared" ref="AJ73:AJ74" si="60">ABS(J73-$M73)</f>
+        <f t="shared" ref="AJ73" si="60">ABS(J73-$M73)</f>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="AK73" s="15">
@@ -11374,15 +11395,15 @@
       <c r="N74" s="68"/>
       <c r="O74" s="68"/>
       <c r="R74" s="4">
-        <f t="shared" ref="R74:R75" si="63">W71</f>
+        <f t="shared" ref="R74" si="63">W71</f>
         <v>933</v>
       </c>
       <c r="S74" s="4">
-        <f t="shared" ref="S74:S75" si="64">AVERAGE(D71:D74)</f>
+        <f t="shared" ref="S74" si="64">AVERAGE(D71:D74)</f>
         <v>665</v>
       </c>
       <c r="T74" s="7">
-        <f t="shared" ref="T74:T75" si="65">S74/S70</f>
+        <f t="shared" ref="T74" si="65">S74/S70</f>
         <v>0.9339887640449438</v>
       </c>
       <c r="U74" s="5">
@@ -13422,7 +13443,7 @@
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -13472,10 +13493,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6"/>
@@ -13485,692 +13506,713 @@
     <col min="4" max="4" width="12.53515625" style="53" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:3">
       <c r="A2" s="29" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:3">
       <c r="A3" s="29" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:3">
       <c r="A4" s="29" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="29" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="69" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="69" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="29" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="29"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="29" t="s">
+    <row r="8" spans="1:3">
+      <c r="A8" s="29"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="29"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="29" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="37">
+    <row r="11" spans="1:3">
+      <c r="A11" s="37">
         <v>43968</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B11" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="41"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="37"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="41"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="29"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="29" t="s">
+      <c r="C11" s="41"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="C12" s="41"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="29"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="29" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="26" t="s">
+    <row r="15" spans="1:3">
+      <c r="A15" s="26" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="26" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="B14" s="26"/>
-      <c r="C14" s="41"/>
-    </row>
-    <row r="15" spans="1:4" s="50" customFormat="1" ht="46.3" customHeight="1">
-      <c r="A15" s="48" t="s">
+    <row r="16" spans="1:3">
+      <c r="A16" s="26" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="B17" s="26"/>
+      <c r="C17" s="41"/>
+    </row>
+    <row r="18" spans="1:4" s="50" customFormat="1" ht="46.3" customHeight="1">
+      <c r="A18" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="48" t="s">
+      <c r="B18" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="49" t="s">
+      <c r="C18" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="D15" s="54" t="s">
+      <c r="D18" s="54" t="s">
         <v>101</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="42" t="s">
-        <v>97</v>
-      </c>
-      <c r="D16" s="55" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="43" t="s">
-        <v>97</v>
-      </c>
-      <c r="D17" s="55" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="42" t="s">
-        <v>97</v>
-      </c>
-      <c r="D18" s="55" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>10</v>
+        <v>57</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>9</v>
       </c>
       <c r="C19" s="42" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D19" s="55" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="42" t="s">
-        <v>98</v>
+        <v>62</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="43" t="s">
+        <v>97</v>
       </c>
       <c r="D20" s="55" t="s">
-        <v>153</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>96</v>
+        <v>63</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>5</v>
       </c>
       <c r="C21" s="42" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D21" s="55" t="s">
-        <v>153</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="26" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C22" s="42" t="s">
         <v>98</v>
       </c>
       <c r="D22" s="55" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="26" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="C23" s="42" t="s">
         <v>98</v>
       </c>
       <c r="D23" s="55" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="26" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>1</v>
+        <v>96</v>
       </c>
       <c r="C24" s="42" t="s">
         <v>98</v>
       </c>
       <c r="D24" s="55" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C25" s="42" t="s">
         <v>98</v>
       </c>
       <c r="D25" s="55" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="26" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>94</v>
+        <v>0</v>
       </c>
       <c r="C26" s="42" t="s">
         <v>98</v>
       </c>
       <c r="D26" s="55" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="26" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>95</v>
+        <v>1</v>
       </c>
       <c r="C27" s="42" t="s">
         <v>98</v>
       </c>
       <c r="D27" s="55" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="26" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>121</v>
+        <v>6</v>
       </c>
       <c r="C28" s="42" t="s">
         <v>98</v>
       </c>
       <c r="D28" s="55" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="B29" s="67" t="s">
-        <v>124</v>
+        <v>61</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>94</v>
       </c>
       <c r="C29" s="42" t="s">
         <v>98</v>
       </c>
       <c r="D29" s="55" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="B30" s="67" t="s">
-        <v>125</v>
+        <v>69</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>95</v>
       </c>
       <c r="C30" s="42" t="s">
         <v>98</v>
       </c>
       <c r="D30" s="55" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="B31" t="s">
-        <v>120</v>
-      </c>
-      <c r="C31" s="40" t="s">
-        <v>97</v>
+        <v>70</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="C31" s="42" t="s">
+        <v>98</v>
       </c>
       <c r="D31" s="55" t="s">
-        <v>137</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="B32" t="s">
-        <v>138</v>
-      </c>
-      <c r="C32" s="40" t="s">
-        <v>139</v>
+        <v>71</v>
+      </c>
+      <c r="B32" s="67" t="s">
+        <v>124</v>
+      </c>
+      <c r="C32" s="42" t="s">
+        <v>98</v>
       </c>
       <c r="D32" s="55" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="B33" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C33" s="43" t="s">
-        <v>97</v>
+        <v>72</v>
+      </c>
+      <c r="B33" s="67" t="s">
+        <v>125</v>
+      </c>
+      <c r="C33" s="42" t="s">
+        <v>98</v>
       </c>
       <c r="D33" s="55" t="s">
-        <v>119</v>
+        <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="B34" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" t="s">
+        <v>120</v>
+      </c>
+      <c r="C34" s="40" t="s">
         <v>97</v>
       </c>
       <c r="D34" s="55" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="B35" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="C35" s="44" t="s">
-        <v>98</v>
+        <v>74</v>
+      </c>
+      <c r="B35" t="s">
+        <v>138</v>
+      </c>
+      <c r="C35" s="40" t="s">
+        <v>139</v>
       </c>
       <c r="D35" s="55" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="B36" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C36" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" s="43" t="s">
         <v>97</v>
       </c>
       <c r="D36" s="55" t="s">
-        <v>4</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="B37" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" s="43" t="s">
         <v>97</v>
       </c>
       <c r="D37" s="55" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="B38" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="C38" s="43" t="s">
-        <v>97</v>
+        <v>76</v>
+      </c>
+      <c r="B38" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" s="44" t="s">
+        <v>98</v>
       </c>
       <c r="D38" s="55" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="B39" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="45" t="s">
         <v>97</v>
       </c>
       <c r="D39" s="55" t="s">
-        <v>107</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="B40" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="C40" s="40" t="s">
-        <v>139</v>
+        <v>78</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="42" t="s">
+        <v>97</v>
       </c>
       <c r="D40" s="55" t="s">
-        <v>141</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="B41" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C41" s="42" t="s">
-        <v>98</v>
+        <v>79</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" s="43" t="s">
+        <v>97</v>
       </c>
       <c r="D41" s="55" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="B42" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C42" s="44" t="s">
-        <v>98</v>
+        <v>80</v>
+      </c>
+      <c r="B42" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="42" t="s">
+        <v>97</v>
       </c>
       <c r="D42" s="55" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="26" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="C43" s="42" t="s">
-        <v>98</v>
+        <v>123</v>
+      </c>
+      <c r="C43" s="40" t="s">
+        <v>139</v>
       </c>
       <c r="D43" s="55" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="26" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="C44" s="42" t="s">
         <v>98</v>
       </c>
       <c r="D44" s="55" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="B45" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="C45" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="B45" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="44" t="s">
         <v>98</v>
       </c>
       <c r="D45" s="55" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="26" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B46" s="18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C46" s="42" t="s">
         <v>98</v>
       </c>
       <c r="D46" s="55" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="26" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C47" s="42" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D47" s="55" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="B48" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C48" s="44" t="s">
-        <v>97</v>
+        <v>86</v>
+      </c>
+      <c r="B48" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="C48" s="42" t="s">
+        <v>98</v>
       </c>
       <c r="D48" s="55" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="26" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C49" s="42" t="s">
         <v>98</v>
       </c>
       <c r="D49" s="55" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="D50" s="55" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B51" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="D51" s="55" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B52" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C52" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="D52" s="55" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="B50" s="18" t="s">
+      <c r="B53" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C50" s="42" t="s">
+      <c r="C53" s="42" t="s">
         <v>98</v>
       </c>
-      <c r="D50" s="55" t="s">
+      <c r="D53" s="55" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="26"/>
-      <c r="B51" s="18"/>
-      <c r="C51" s="42"/>
-      <c r="D51" s="55"/>
-    </row>
-    <row r="52" spans="1:4" s="29" customFormat="1">
-      <c r="A52" s="29" t="s">
+    <row r="54" spans="1:4">
+      <c r="A54" s="26"/>
+      <c r="B54" s="18"/>
+      <c r="C54" s="42"/>
+      <c r="D54" s="55"/>
+    </row>
+    <row r="55" spans="1:4" s="29" customFormat="1">
+      <c r="A55" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="B52" s="51"/>
-      <c r="C52" s="52"/>
-      <c r="D52" s="54"/>
-    </row>
-    <row r="53" spans="1:4" s="50" customFormat="1" ht="46.3" customHeight="1">
-      <c r="A53" s="48" t="s">
+      <c r="B55" s="51"/>
+      <c r="C55" s="52"/>
+      <c r="D55" s="54"/>
+    </row>
+    <row r="56" spans="1:4" s="50" customFormat="1" ht="46.3" customHeight="1">
+      <c r="A56" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="B53" s="48" t="s">
+      <c r="B56" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="C53" s="49"/>
-      <c r="D53" s="54"/>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="B54" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="C54" s="26"/>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="26" t="s">
-        <v>142</v>
-      </c>
-      <c r="B55" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="C55" s="47"/>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="B56" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="C56" s="44"/>
+      <c r="C56" s="49"/>
+      <c r="D56" s="54"/>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="B57" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="C57" s="42"/>
+        <v>92</v>
+      </c>
+      <c r="B57" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C57" s="26"/>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="26" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B58" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="C58" s="46"/>
+        <v>133</v>
+      </c>
+      <c r="C58" s="47"/>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="26" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B59" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="C59" s="46"/>
+        <v>134</v>
+      </c>
+      <c r="C59" s="44"/>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="26" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B60" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="C60" s="46"/>
+        <v>135</v>
+      </c>
+      <c r="C60" s="42"/>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="26" t="s">
-        <v>148</v>
-      </c>
-      <c r="B61" s="17" t="s">
-        <v>126</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="B61" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="C61" s="46"/>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="B62" s="17" t="s">
-        <v>43</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="B62" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="C62" s="46"/>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="B63" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="C63" s="46"/>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="B64" s="17" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="B65" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="B63" s="17" t="s">
+      <c r="B66" s="17" t="s">
         <v>44</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A5" r:id="rId1"/>
+    <hyperlink ref="A6" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>